<commit_message>
Direct comparison of acceptance rates
</commit_message>
<xml_diff>
--- a/examples/emulators/mcmc/figures/nn-6-64-50000.xlsx
+++ b/examples/emulators/mcmc/figures/nn-6-64-50000.xlsx
@@ -462,37 +462,37 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>0.7600706313028855</v>
+        <v>0.7723323445918061</v>
       </c>
       <c r="C2">
-        <v>0.02980113005507119</v>
+        <v>0.03445658242777255</v>
       </c>
       <c r="D2">
-        <v>0.741284663905331</v>
+        <v>0.7420760148450991</v>
       </c>
       <c r="E2">
-        <v>0.7460651726663367</v>
+        <v>0.7470135935518118</v>
       </c>
       <c r="F2">
-        <v>0.748735913144807</v>
+        <v>0.7504261789608688</v>
       </c>
       <c r="G2">
-        <v>0.7521221130745408</v>
+        <v>0.815963055533745</v>
       </c>
       <c r="H2">
-        <v>0.8370561978342003</v>
+        <v>0.8285271493034808</v>
       </c>
       <c r="I2">
-        <v>2.493054900545754</v>
+        <v>12.16421095134998</v>
       </c>
       <c r="J2">
-        <v>918.9420611280607</v>
+        <v>141.3751908297425</v>
       </c>
       <c r="K2">
-        <v>5.831173589574624</v>
+        <v>2.085189552194268</v>
       </c>
       <c r="L2">
-        <v>157.5912716388702</v>
+        <v>67.79968309402466</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -500,37 +500,37 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>1.010592485266492</v>
+        <v>1.029607109549036</v>
       </c>
       <c r="C3">
-        <v>0.03474293078860247</v>
+        <v>0.0432930973429417</v>
       </c>
       <c r="D3">
-        <v>0.989291922634672</v>
+        <v>0.9924916943952069</v>
       </c>
       <c r="E3">
-        <v>0.994370102741551</v>
+        <v>0.9978198610884508</v>
       </c>
       <c r="F3">
-        <v>0.9973544562926941</v>
+        <v>1.001742467856205</v>
       </c>
       <c r="G3">
-        <v>1.000780555800823</v>
+        <v>1.085878115265738</v>
       </c>
       <c r="H3">
-        <v>1.097947423001483</v>
+        <v>1.098446944070902</v>
       </c>
       <c r="I3">
-        <v>2.647759885687017</v>
+        <v>13.77736584698096</v>
       </c>
       <c r="J3">
-        <v>364.9186389267174</v>
+        <v>734.7185699630767</v>
       </c>
       <c r="K3">
-        <v>2.315601842232418</v>
+        <v>10.83660773080854</v>
       </c>
       <c r="L3">
-        <v>157.5912716388702</v>
+        <v>67.79968309402466</v>
       </c>
     </row>
   </sheetData>

</xml_diff>